<commit_message>
Add fundamentals module and add to main
</commit_message>
<xml_diff>
--- a/V2/Final-Project-Plan.xlsx
+++ b/V2/Final-Project-Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca-my.sharepoint.com/personal/adsmith6_myseneca_ca/Documents/CPR101/finalProject/project/git/CPR101group3/V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{40108199-1571-4FD1-AE3A-D7CA79A9ACE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E516C198-16D7-4852-B39E-685A567A3728}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{40108199-1571-4FD1-AE3A-D7CA79A9ACE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8A311EC-A2FB-4286-8E3C-D9AE24553BF7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D8E31B3C-F149-45D6-99B7-2CDC65D256FF}"/>
   </bookViews>
@@ -638,7 +638,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
   <si>
     <t>Blackboard Group No
 3 Class NAA</t>
@@ -938,23 +938,6 @@
 see Project Milestones and Details page, "Request review of a file..."</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Axton Smith
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Fundamentals</t>
-    </r>
-  </si>
-  <si>
     <t>Review each other's PM notes on process Teams. Agree on how project will be done.
 Decide which module to do
 &amp; choose Team Leader</t>
@@ -1215,10 +1198,27 @@
     <t>Add string comparions module and pushed to github.</t>
   </si>
   <si>
-    <t>Add converting to doubles module and push to github.</t>
-  </si>
-  <si>
     <t>Module written into the source code, test cases written and ran, module pushed to github.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Damian Orfao
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fundamentals</t>
+    </r>
+  </si>
+  <si>
+    <t>Add converting to doubles module and push to github, add all other modules to main and push to github.</t>
   </si>
 </sst>
 </file>
@@ -1707,27 +1707,27 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2356,10 +2356,10 @@
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomRight" activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2396,41 +2396,41 @@
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50" t="s">
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="51" t="s">
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="48" t="s">
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
@@ -2844,13 +2844,13 @@
     </row>
     <row r="7" spans="1:26" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="C7" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="D7" s="11">
         <v>2</v>
@@ -2865,10 +2865,10 @@
         <v>29</v>
       </c>
       <c r="G7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="I7" s="11">
         <v>2</v>
@@ -2883,7 +2883,7 @@
         <v>29</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="P7" s="17"/>
       <c r="Q7" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R7" s="17"/>
       <c r="S7" s="17"/>
@@ -2920,13 +2920,13 @@
     </row>
     <row r="8" spans="1:26" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="D8" s="43">
         <v>2</v>
@@ -2941,10 +2941,10 @@
         <v>29</v>
       </c>
       <c r="G8" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>46</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>47</v>
       </c>
       <c r="I8" s="11">
         <v>3</v>
@@ -2958,11 +2958,11 @@
       <c r="K8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="54" t="s">
+      <c r="L8" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="M8" s="17" t="s">
-        <v>65</v>
       </c>
       <c r="N8" s="17">
         <v>1</v>
@@ -2977,7 +2977,7 @@
         <v>29</v>
       </c>
       <c r="Q8" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="9" spans="1:26" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="D9" s="11">
         <v>2</v>
@@ -3023,10 +3023,10 @@
         <v>22</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I9" s="11">
         <v>2</v>
@@ -3041,7 +3041,7 @@
         <v>29</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="P9" s="17"/>
       <c r="Q9" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
@@ -3078,13 +3078,13 @@
     </row>
     <row r="10" spans="1:26" s="15" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="D10" s="11">
         <v>4</v>
@@ -3096,13 +3096,13 @@
 Dec.1</v>
       </c>
       <c r="F10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="H10" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="I10" s="11">
         <v>3</v>
@@ -3116,11 +3116,11 @@
       <c r="K10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="54" t="s">
-        <v>64</v>
+      <c r="L10" s="48" t="s">
+        <v>65</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N10" s="11">
         <v>2</v>
@@ -3131,9 +3131,11 @@
         <v>Monday
 Dec.11</v>
       </c>
-      <c r="P10" s="11"/>
+      <c r="P10" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="Q10" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
@@ -3158,19 +3160,19 @@
     </row>
     <row r="11" spans="1:26" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="O11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="T11" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="O11" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="T11" s="25" t="s">
+      <c r="Y11" s="27" t="s">
         <v>56</v>
-      </c>
-      <c r="Y11" s="27" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="13" customFormat="1" ht="240" x14ac:dyDescent="0.25">
@@ -3178,10 +3180,10 @@
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>58</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>59</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
@@ -3191,12 +3193,12 @@
       <c r="P12" s="18"/>
       <c r="S12" s="18"/>
       <c r="T12" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U12" s="18"/>
       <c r="X12" s="18"/>
       <c r="Y12" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Z12" s="18"/>
     </row>
@@ -3362,21 +3364,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B0151594D7FCB5488E5A9E489924D9EC" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="782c9240cb3ad67681d064f8c60b5904">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="704fc4e2-c222-4319-b029-9522ae630171" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb47d0c3166dea3cfdc3792473b57f5a" ns2:_="">
     <xsd:import namespace="704fc4e2-c222-4319-b029-9522ae630171"/>
@@ -3514,24 +3501,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76FEA26C-2233-4295-8BE1-B265CEAD26C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A37522F-39F4-4439-AEEC-7D6E0C35C759}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{877BC3CA-6C3C-4A4E-AA42-8A543635C4C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3547,4 +3532,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A37522F-39F4-4439-AEEC-7D6E0C35C759}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76FEA26C-2233-4295-8BE1-B265CEAD26C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>